<commit_message>
CollisionListener for enemyMissiles <-> shooters
</commit_message>
<xml_diff>
--- a/CollisionsMatrix.xlsx
+++ b/CollisionsMatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolvisser/Workspace/cse214-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA94B50-CAE0-F345-A6E2-751A361B7362}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12C2F88-E307-B947-86F6-703636F5B555}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{8C2B8C3C-353B-8547-96D3-1BC8BF249FD3}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{8C2B8C3C-353B-8547-96D3-1BC8BF249FD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="16">
   <si>
     <t>Shooter</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Assume not possible</t>
+  </si>
+  <si>
+    <t>As implemented in game via CollisionListener</t>
   </si>
 </sst>
 </file>
@@ -108,7 +111,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -136,6 +139,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -167,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -179,6 +188,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,15 +504,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0E3CA8F-51AD-EC42-B793-E55261AA00DF}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29.5" bestFit="1" customWidth="1"/>
@@ -627,6 +639,134 @@
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="9"/>
     </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="11" t="str">
+        <f>D11</f>
+        <v>Shooter takes damage, missile explodes</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="11" t="str">
+        <f>E11</f>
+        <v>Equip</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
CollisionListener for enemyMissiles <-> shooterMissiles [NOT IDEAL]
more
</commit_message>
<xml_diff>
--- a/CollisionsMatrix.xlsx
+++ b/CollisionsMatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolvisser/Workspace/cse214-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12C2F88-E307-B947-86F6-703636F5B555}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFCD0CD-15A1-2A43-9A5D-BAFEB2FEECD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{8C2B8C3C-353B-8547-96D3-1BC8BF249FD3}"/>
   </bookViews>
@@ -507,13 +507,14 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.33203125" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29.5" bestFit="1" customWidth="1"/>
@@ -692,7 +693,7 @@
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="11" t="s">
         <v>12</v>
       </c>
       <c r="E12" s="1" t="s">
@@ -713,7 +714,10 @@
         <f>D11</f>
         <v>Shooter takes damage, missile explodes</v>
       </c>
-      <c r="C13" s="6"/>
+      <c r="C13" s="11" t="str">
+        <f>D12</f>
+        <v>Both explode</v>
+      </c>
       <c r="D13" s="6"/>
       <c r="E13" s="2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
CollisionListener for shooterMissiles <-> powerUps
</commit_message>
<xml_diff>
--- a/CollisionsMatrix.xlsx
+++ b/CollisionsMatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolvisser/Workspace/cse214-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFCD0CD-15A1-2A43-9A5D-BAFEB2FEECD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71BA3D2-9B87-4B4A-9E2D-81E79912A8F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{8C2B8C3C-353B-8547-96D3-1BC8BF249FD3}"/>
   </bookViews>
@@ -507,7 +507,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -515,7 +515,7 @@
     <col min="1" max="1" width="33.33203125" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -696,7 +696,7 @@
       <c r="D12" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="11" t="s">
         <v>8</v>
       </c>
       <c r="F12" s="1" t="s">
@@ -737,7 +737,10 @@
         <f>E11</f>
         <v>Equip</v>
       </c>
-      <c r="C14" s="6"/>
+      <c r="C14" s="11" t="str">
+        <f>E12</f>
+        <v>Equip</v>
+      </c>
       <c r="D14" s="7"/>
       <c r="E14" s="6"/>
       <c r="F14" s="3" t="s">

</xml_diff>

<commit_message>
CollisionListener for bunker <-> missiles (enemy and shooter)
update excel
</commit_message>
<xml_diff>
--- a/CollisionsMatrix.xlsx
+++ b/CollisionsMatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolvisser/Workspace/cse214-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71BA3D2-9B87-4B4A-9E2D-81E79912A8F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D220C42-CFD9-1B42-BE66-308348E81CC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{8C2B8C3C-353B-8547-96D3-1BC8BF249FD3}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="16">
   <si>
     <t>Shooter</t>
   </si>
@@ -176,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -190,6 +190,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,14 +508,14 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.33203125" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29.5" bestFit="1" customWidth="1"/>
@@ -691,7 +692,9 @@
       <c r="A12" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="6"/>
+      <c r="B12" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="C12" s="6"/>
       <c r="D12" s="11" t="s">
         <v>12</v>
@@ -702,7 +705,7 @@
       <c r="F12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="11" t="s">
         <v>13</v>
       </c>
     </row>
@@ -725,7 +728,7 @@
       <c r="F13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="11" t="s">
         <v>13</v>
       </c>
     </row>
@@ -741,7 +744,9 @@
         <f>E12</f>
         <v>Equip</v>
       </c>
-      <c r="D14" s="7"/>
+      <c r="D14" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E14" s="6"/>
       <c r="F14" s="3" t="s">
         <v>6</v>
@@ -754,10 +759,14 @@
       <c r="A15" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="F15" s="6"/>
       <c r="G15" s="5" t="s">
         <v>7</v>
@@ -767,11 +776,23 @@
       <c r="A16" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
+      <c r="B16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="11" t="str">
+        <f>G12</f>
+        <v>Missile bursts and removes blocks</v>
+      </c>
+      <c r="D16" s="11" t="str">
+        <f>G13</f>
+        <v>Missile bursts and removes blocks</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="G16" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CollisionListener for enemyWave <-> shooterMissiles
</commit_message>
<xml_diff>
--- a/CollisionsMatrix.xlsx
+++ b/CollisionsMatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolvisser/Workspace/cse214-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D220C42-CFD9-1B42-BE66-308348E81CC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB65A2F8-1A69-2D4B-8F81-E0769029B889}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{8C2B8C3C-353B-8547-96D3-1BC8BF249FD3}"/>
   </bookViews>
@@ -702,7 +702,7 @@
       <c r="E12" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G12" s="11" t="s">
@@ -760,7 +760,10 @@
         <v>4</v>
       </c>
       <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
+      <c r="C15" s="11" t="str">
+        <f>F12</f>
+        <v>Enemy takes damage, missile explodes</v>
+      </c>
       <c r="D15" s="4" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
CollisionListener for enemyWave <-> Shooter; plus other rewriting to be more neat
</commit_message>
<xml_diff>
--- a/CollisionsMatrix.xlsx
+++ b/CollisionsMatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolvisser/Workspace/cse214-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB65A2F8-1A69-2D4B-8F81-E0769029B889}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E30701F-FEF1-9540-BE1E-D431EE5159F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{8C2B8C3C-353B-8547-96D3-1BC8BF249FD3}"/>
   </bookViews>
@@ -176,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -190,7 +190,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,7 +507,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -681,7 +680,7 @@
       <c r="E11" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="11" t="s">
         <v>10</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -759,7 +758,10 @@
       <c r="A15" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="13"/>
+      <c r="B15" s="11" t="str">
+        <f>F11</f>
+        <v>Kills Shooter</v>
+      </c>
       <c r="C15" s="11" t="str">
         <f>F12</f>
         <v>Enemy takes damage, missile explodes</v>

</xml_diff>